<commit_message>
Debt Case Manageemnt Local Execution merged with regression Feb02
</commit_message>
<xml_diff>
--- a/src/test/resources/docs/BankFile.xlsx
+++ b/src/test/resources/docs/BankFile.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Bank Name:</t>
   </si>
@@ -115,6 +115,18 @@
   </si>
   <si>
     <t>7.848.00</t>
+  </si>
+  <si>
+    <t>01-25-2019 17:17:10</t>
+  </si>
+  <si>
+    <t>FT19012500004</t>
+  </si>
+  <si>
+    <t>20190125044036506</t>
+  </si>
+  <si>
+    <t>Regression daysixtw</t>
   </si>
 </sst>
 </file>
@@ -607,19 +619,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="I7" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
updated code with user registration
</commit_message>
<xml_diff>
--- a/src/test/resources/docs/BankFile.xlsx
+++ b/src/test/resources/docs/BankFile.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
   <si>
     <t>Bank Name:</t>
   </si>
@@ -127,6 +127,24 @@
   </si>
   <si>
     <t>Regression daysixtw</t>
+  </si>
+  <si>
+    <t>02-19-2019 18:51:51</t>
+  </si>
+  <si>
+    <t>FT19021900039</t>
+  </si>
+  <si>
+    <t>20190219041910569</t>
+  </si>
+  <si>
+    <t>Automation FIftyfour</t>
+  </si>
+  <si>
+    <t>02-19-2019 18:57:57</t>
+  </si>
+  <si>
+    <t>FT19021900040</t>
   </si>
 </sst>
 </file>
@@ -619,19 +637,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I7" t="s">
         <v>29</v>

</xml_diff>